<commit_message>
merged and sorted excel sheets after data collection
</commit_message>
<xml_diff>
--- a/output/execution_times/R/execution_times_R_small.xlsx
+++ b/output/execution_times/R/execution_times_R_small.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Method</t>
   </si>
@@ -122,6 +122,42 @@
   </si>
   <si>
     <t xml:space="preserve">2025-04-12 16:09:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 16:06:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-04-12 23:46:40</t>
   </si>
 </sst>
 </file>
@@ -466,189 +502,206 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>1.6648690700530999</v>
+        <v>1.6648690700531</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
         <v>1.69384098052979</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C4" t="n">
         <v>1.69663906097412</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C5" t="n">
-        <v>1.6830201148986801</v>
+        <v>1.68302011489868</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C6" t="n">
-        <v>1.6802401542663601</v>
+        <v>1.68024015426636</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C7" t="n">
-        <v>1.6844108104705799</v>
+        <v>1.68441081047058</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C8" t="n">
-        <v>1.6866028308868399</v>
+        <v>1.68660283088684</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C9" t="n">
         <v>1.70475196838379</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C10" t="n">
-        <v>1.6944098472595199</v>
+        <v>1.69440984725952</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C11" t="n">
         <v>1.66802501678467</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="n">
+        <v>14.4005200862885</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>